<commit_message>
spring jpa jdbc updated
</commit_message>
<xml_diff>
--- a/InterviewTopics.xlsx
+++ b/InterviewTopics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HK\docs\study\Interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8C0D56E-C3BF-4913-8F38-2D4EF7FB7C9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FA8216-9920-47DC-989B-9935EDB8021A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>Topic</t>
   </si>
@@ -134,12 +134,33 @@
   </si>
   <si>
     <t>CSS</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>Thread</t>
+  </si>
+  <si>
+    <t>Oauth 2</t>
+  </si>
+  <si>
+    <t>yet to start</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -973,14 +994,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -996,170 +1022,225 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="F18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="F19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="F31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="F32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="F33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>37</v>
+      </c>
+      <c r="F34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>